<commit_message>
Updated data and scripts
</commit_message>
<xml_diff>
--- a/genlang_all_cohorts_updated.xlsx
+++ b/genlang_all_cohorts_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/sp58_st-andrews_ac_uk/Documents/gen_lang_hand_meta/Old/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="665" documentId="13_ncr:1_{0B6902DA-2242-D64D-8D8C-45B1C2605456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F2E6B79-191E-E247-9DC8-8786F817D4AB}"/>
+  <xr:revisionPtr revIDLastSave="748" documentId="13_ncr:1_{0B6902DA-2242-D64D-8D8C-45B1C2605456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{777930A4-45C5-4D4D-A9D3-EC0D66683214}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="520" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{A6332151-AACC-E14E-B3DF-3D4980E70093}"/>
+    <workbookView xWindow="-7120" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{A6332151-AACC-E14E-B3DF-3D4980E70093}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined2" sheetId="12" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="140">
   <si>
     <t xml:space="preserve">TD Left-Handers </t>
   </si>
@@ -727,11 +727,29 @@
   <si>
     <t>Manchester (OLD)</t>
   </si>
+  <si>
+    <t>ALSPAC controls with child.therapy</t>
+  </si>
+  <si>
+    <t>MANCHESTER</t>
+  </si>
+  <si>
+    <t>Total RD - NTR/NeuroDys</t>
+  </si>
+  <si>
+    <t>Total controls - NTR/NeuroDys</t>
+  </si>
+  <si>
+    <t>Tot Case + control (no NTR&lt;…)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -926,7 +944,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -943,6 +961,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1081,7 +1105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1204,8 +1228,29 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1225,23 +1270,8 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1262,19 +1292,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1594,7 +1634,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1685,11 +1725,11 @@
       </c>
       <c r="D4" s="5">
         <f>Check_16052021!$H$11</f>
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="E4" s="5">
         <f>Check_16052021!$J$11</f>
-        <v>1931</v>
+        <v>1375</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
@@ -1732,11 +1772,11 @@
       </c>
       <c r="D6" s="5">
         <f>Check_16052021!H32</f>
-        <v>188</v>
+        <v>135</v>
       </c>
       <c r="E6" s="5">
         <f>Check_16052021!J32</f>
-        <v>1442</v>
+        <v>1026</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>23</v>
@@ -1754,11 +1794,11 @@
       </c>
       <c r="D7" s="5">
         <f>Check_16052021!$H$41</f>
-        <v>197</v>
+        <v>144</v>
       </c>
       <c r="E7" s="5">
         <f>Check_16052021!$J$41</f>
-        <v>1623</v>
+        <v>1156</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>23</v>
@@ -1885,11 +1925,11 @@
       </c>
       <c r="D2" s="5">
         <f>Check_16052021!$H$40</f>
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E2" s="5">
         <f>Check_16052021!$J$40</f>
-        <v>522</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1927,11 +1967,11 @@
       </c>
       <c r="D4" s="5">
         <f>Check_16052021!$H$10</f>
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5">
         <f>Check_16052021!$J$10</f>
-        <v>830</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1999,11 +2039,11 @@
       </c>
       <c r="D2" s="5">
         <f>Check_16052021!$H$39</f>
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="E2" s="5">
         <f>Check_16052021!$J$39</f>
-        <v>1101</v>
+        <v>784</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2041,11 +2081,11 @@
       </c>
       <c r="D4" s="5">
         <f>Check_16052021!H3</f>
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="E4" s="5">
         <f>Check_16052021!J3</f>
-        <v>1101</v>
+        <v>784</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2130,16 +2170,16 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
       <c r="J2" t="s">
         <v>87</v>
       </c>
@@ -2294,16 +2334,16 @@
       <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:19" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
       <c r="J7" t="s">
         <v>90</v>
       </c>
@@ -6011,11 +6051,11 @@
       </c>
       <c r="D4" s="5">
         <f>Check_16052021!$H$10</f>
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5">
         <f>Check_16052021!$J$10</f>
-        <v>830</v>
+        <v>591</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
@@ -6058,11 +6098,11 @@
       </c>
       <c r="D6" s="5">
         <f>Check_16052021!$H$31</f>
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E6" s="5">
         <f>Check_16052021!$J$31</f>
-        <v>341</v>
+        <v>242</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>23</v>
@@ -6081,11 +6121,11 @@
       </c>
       <c r="D7" s="5">
         <f>Check_16052021!$H$40</f>
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E7" s="5">
         <f>Check_16052021!$J$40</f>
-        <v>522</v>
+        <v>372</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>23</v>
@@ -6124,7 +6164,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6211,11 +6251,11 @@
       </c>
       <c r="D4" s="5">
         <f>Check_16052021!$H$9</f>
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="E4" s="5">
         <f>Check_16052021!$J$9</f>
-        <v>1101</v>
+        <v>784</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
@@ -6256,11 +6296,11 @@
       </c>
       <c r="D6" s="5">
         <f>Check_16052021!$H$30</f>
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="E6" s="5">
         <f>Check_16052021!$J$30</f>
-        <v>1101</v>
+        <v>784</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>23</v>
@@ -6279,11 +6319,11 @@
       </c>
       <c r="D7" s="5">
         <f>Check_16052021!$H$39</f>
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="E7" s="5">
         <f>Check_16052021!$J$39</f>
-        <v>1101</v>
+        <v>784</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>23</v>
@@ -6436,15 +6476,15 @@
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72" t="s">
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="P5" s="72"/>
+      <c r="P5" s="73"/>
       <c r="Q5" s="11" t="s">
         <v>74</v>
       </c>
@@ -6666,15 +6706,15 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="L11" s="72" t="s">
+      <c r="L11" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="72" t="s">
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="72"/>
+      <c r="P11" s="73"/>
       <c r="Q11" s="11" t="s">
         <v>74</v>
       </c>
@@ -7161,8 +7201,8 @@
   <dimension ref="A1:Q97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48:J50"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7173,42 +7213,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="92"/>
+      <c r="F1" s="93"/>
       <c r="G1" s="52"/>
-      <c r="H1" s="92" t="s">
+      <c r="H1" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="92"/>
+      <c r="I1" s="93"/>
       <c r="J1" s="52"/>
-      <c r="K1" s="91" t="s">
+      <c r="K1" s="86" t="s">
         <v>133</v>
       </c>
-      <c r="L1" s="91"/>
+      <c r="L1" s="86"/>
       <c r="M1" s="59"/>
       <c r="N1" s="59"/>
       <c r="O1" s="59"/>
       <c r="P1" s="59"/>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
       <c r="E2" s="57" t="s">
         <v>106</v>
       </c>
@@ -7247,13 +7287,13 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="90" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="62" t="s">
@@ -7270,14 +7310,14 @@
         <v>54</v>
       </c>
       <c r="H3" s="65">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="I3" s="65">
-        <v>955</v>
+        <v>678</v>
       </c>
       <c r="J3" s="62">
         <f>H3+I3</f>
-        <v>1101</v>
+        <v>784</v>
       </c>
       <c r="K3" s="62">
         <v>0.17</v>
@@ -7289,9 +7329,9 @@
         <f>E3/(F3+E3)</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="N3" s="60">
+      <c r="N3" s="97">
         <f t="shared" ref="N3:N40" si="0">H3/J3</f>
-        <v>0.13260672116257946</v>
+        <v>0.13520408163265307</v>
       </c>
       <c r="O3" s="64">
         <v>1.11111111</v>
@@ -7301,9 +7341,9 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
+      <c r="A4" s="88"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
       <c r="D4" s="66" t="s">
         <v>42</v>
       </c>
@@ -7318,14 +7358,14 @@
         <v>60</v>
       </c>
       <c r="H4" s="66">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="I4" s="66">
-        <v>742</v>
+        <v>528</v>
       </c>
       <c r="J4" s="62">
         <f t="shared" ref="J4:J50" si="2">H4+I4</f>
-        <v>830</v>
+        <v>591</v>
       </c>
       <c r="K4" s="66">
         <v>0.11</v>
@@ -7339,15 +7379,15 @@
       </c>
       <c r="N4" s="60">
         <f t="shared" si="0"/>
-        <v>0.10602409638554217</v>
+        <v>0.1065989847715736</v>
       </c>
       <c r="O4" s="64"/>
       <c r="P4" s="64"/>
     </row>
     <row r="5" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="86"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="90"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="92"/>
       <c r="D5" s="62" t="s">
         <v>43</v>
       </c>
@@ -7363,15 +7403,15 @@
       </c>
       <c r="H5" s="65">
         <f>H3+H4</f>
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="I5" s="65">
         <f>I3+I4</f>
-        <v>1697</v>
+        <v>1206</v>
       </c>
       <c r="J5" s="62">
         <f t="shared" si="2"/>
-        <v>1931</v>
+        <v>1375</v>
       </c>
       <c r="K5" s="62">
         <v>0.14000000000000001</v>
@@ -7385,15 +7425,15 @@
       </c>
       <c r="N5" s="60">
         <f t="shared" si="0"/>
-        <v>0.12118073537027448</v>
+        <v>0.12290909090909091</v>
       </c>
       <c r="O5" s="64"/>
       <c r="P5" s="64"/>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="86"/>
-      <c r="B6" s="89"/>
-      <c r="C6" s="88" t="s">
+      <c r="A6" s="88"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="90" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="66" t="s">
@@ -7409,15 +7449,15 @@
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="H6" s="65">
-        <v>146</v>
-      </c>
-      <c r="I6" s="65">
-        <v>955</v>
+      <c r="H6" s="72">
+        <v>106</v>
+      </c>
+      <c r="I6" s="72">
+        <v>678</v>
       </c>
       <c r="J6" s="62">
         <f t="shared" si="2"/>
-        <v>1101</v>
+        <v>784</v>
       </c>
       <c r="K6" s="66">
         <v>0.11</v>
@@ -7431,7 +7471,7 @@
       </c>
       <c r="N6" s="60">
         <f t="shared" si="0"/>
-        <v>0.13260672116257946</v>
+        <v>0.13520408163265307</v>
       </c>
       <c r="O6" s="64">
         <v>1.44230769</v>
@@ -7441,9 +7481,9 @@
       </c>
     </row>
     <row r="7" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="86"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
       <c r="D7" s="62" t="s">
         <v>42</v>
       </c>
@@ -7458,14 +7498,14 @@
         <v>104</v>
       </c>
       <c r="H7" s="66">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="I7" s="66">
-        <v>742</v>
+        <v>528</v>
       </c>
       <c r="J7" s="62">
         <f t="shared" si="2"/>
-        <v>830</v>
+        <v>591</v>
       </c>
       <c r="K7" s="62">
         <v>0.12</v>
@@ -7479,15 +7519,15 @@
       </c>
       <c r="N7" s="60">
         <f t="shared" si="0"/>
-        <v>0.10602409638554217</v>
+        <v>0.1065989847715736</v>
       </c>
       <c r="O7" s="64"/>
       <c r="P7" s="64"/>
     </row>
     <row r="8" spans="1:17" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="86"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="90"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="92"/>
       <c r="D8" s="66" t="s">
         <v>43</v>
       </c>
@@ -7501,17 +7541,17 @@
         <f t="shared" si="1"/>
         <v>254</v>
       </c>
-      <c r="H8" s="65">
+      <c r="H8" s="72">
         <f>H6+H7</f>
-        <v>234</v>
-      </c>
-      <c r="I8" s="65">
+        <v>169</v>
+      </c>
+      <c r="I8" s="72">
         <f>I6+I7</f>
-        <v>1697</v>
+        <v>1206</v>
       </c>
       <c r="J8" s="62">
         <f t="shared" si="2"/>
-        <v>1931</v>
+        <v>1375</v>
       </c>
       <c r="K8" s="66">
         <v>0.11</v>
@@ -7525,15 +7565,15 @@
       </c>
       <c r="N8" s="60">
         <f t="shared" si="0"/>
-        <v>0.12118073537027448</v>
+        <v>0.12290909090909091</v>
       </c>
       <c r="O8" s="64"/>
       <c r="P8" s="64"/>
     </row>
     <row r="9" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="86"/>
-      <c r="B9" s="89"/>
-      <c r="C9" s="88" t="s">
+      <c r="A9" s="88"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="90" t="s">
         <v>114</v>
       </c>
       <c r="D9" s="62" t="s">
@@ -7549,15 +7589,15 @@
         <f t="shared" si="1"/>
         <v>210</v>
       </c>
-      <c r="H9" s="65">
-        <v>146</v>
-      </c>
-      <c r="I9" s="65">
-        <v>955</v>
+      <c r="H9" s="98">
+        <v>106</v>
+      </c>
+      <c r="I9" s="98">
+        <v>678</v>
       </c>
       <c r="J9" s="62">
         <f>H9+I9</f>
-        <v>1101</v>
+        <v>784</v>
       </c>
       <c r="K9" s="62">
         <v>0.13</v>
@@ -7571,7 +7611,7 @@
       </c>
       <c r="N9" s="60">
         <f t="shared" si="0"/>
-        <v>0.13260672116257946</v>
+        <v>0.13520408163265307</v>
       </c>
       <c r="O9" s="64">
         <f>G9/G10</f>
@@ -7579,16 +7619,16 @@
       </c>
       <c r="P9" s="64">
         <f>J9/J10</f>
-        <v>1.3265060240963855</v>
+        <v>1.3265651438240271</v>
       </c>
       <c r="Q9" s="5" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="86"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="89"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="66" t="s">
         <v>42</v>
       </c>
@@ -7602,15 +7642,15 @@
         <f t="shared" si="1"/>
         <v>158</v>
       </c>
-      <c r="H10" s="66">
-        <v>88</v>
-      </c>
-      <c r="I10" s="66">
-        <v>742</v>
+      <c r="H10" s="99">
+        <v>63</v>
+      </c>
+      <c r="I10" s="99">
+        <v>528</v>
       </c>
       <c r="J10" s="62">
         <f>H10+I10</f>
-        <v>830</v>
+        <v>591</v>
       </c>
       <c r="K10" s="66">
         <v>0.11</v>
@@ -7624,14 +7664,14 @@
       </c>
       <c r="N10" s="60">
         <f t="shared" si="0"/>
-        <v>0.10602409638554217</v>
+        <v>0.1065989847715736</v>
       </c>
       <c r="P10" s="64"/>
     </row>
     <row r="11" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="87"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="92"/>
       <c r="D11" s="62" t="s">
         <v>43</v>
       </c>
@@ -7647,17 +7687,15 @@
         <f t="shared" si="1"/>
         <v>368</v>
       </c>
-      <c r="H11" s="62">
-        <f>H9+H10</f>
-        <v>234</v>
-      </c>
-      <c r="I11" s="65">
-        <f>I9+I10</f>
-        <v>1697</v>
+      <c r="H11" s="98">
+        <v>169</v>
+      </c>
+      <c r="I11" s="98">
+        <v>1206</v>
       </c>
       <c r="J11" s="62">
         <f>H11+I11</f>
-        <v>1931</v>
+        <v>1375</v>
       </c>
       <c r="K11" s="62">
         <v>0.12</v>
@@ -7671,19 +7709,19 @@
       </c>
       <c r="N11" s="60">
         <f>H11/J11</f>
-        <v>0.12118073537027448</v>
+        <v>0.12290909090909091</v>
       </c>
       <c r="O11" s="64"/>
       <c r="P11" s="64"/>
     </row>
     <row r="12" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="82" t="s">
+      <c r="C12" s="77" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="56" t="s">
@@ -7731,9 +7769,9 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="93"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
       <c r="D13" s="55" t="s">
         <v>42</v>
       </c>
@@ -7775,9 +7813,9 @@
       <c r="P13" s="59"/>
     </row>
     <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="81"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="84"/>
+      <c r="A14" s="76"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="56" t="s">
         <v>43</v>
       </c>
@@ -7821,13 +7859,13 @@
       <c r="P14" s="59"/>
     </row>
     <row r="15" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="76" t="s">
+      <c r="C15" s="83" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="68" t="s">
@@ -7875,9 +7913,9 @@
       </c>
     </row>
     <row r="16" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="84"/>
       <c r="D16" s="67" t="s">
         <v>42</v>
       </c>
@@ -7919,9 +7957,9 @@
       <c r="P16" s="70"/>
     </row>
     <row r="17" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="68" t="s">
         <v>43</v>
       </c>
@@ -7967,13 +8005,13 @@
       <c r="P17" s="70"/>
     </row>
     <row r="18" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="79" t="s">
+      <c r="A18" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="82" t="s">
+      <c r="C18" s="77" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="56" t="s">
@@ -8021,9 +8059,9 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="93"/>
-      <c r="B19" s="94"/>
-      <c r="C19" s="94"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
       <c r="D19" s="55" t="s">
         <v>42</v>
       </c>
@@ -8065,9 +8103,9 @@
       <c r="P19" s="59"/>
     </row>
     <row r="20" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="81"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="84"/>
+      <c r="A20" s="76"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
       <c r="D20" s="56" t="s">
         <v>43</v>
       </c>
@@ -8092,7 +8130,7 @@
         <v>389</v>
       </c>
       <c r="J20" s="55">
-        <f t="shared" si="2"/>
+        <f>H20+I20</f>
         <v>438</v>
       </c>
       <c r="K20" s="56">
@@ -8113,13 +8151,13 @@
       <c r="P20" s="59"/>
     </row>
     <row r="21" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="79" t="s">
+      <c r="A21" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="77" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="55" t="s">
@@ -8167,9 +8205,9 @@
       </c>
     </row>
     <row r="22" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="93"/>
-      <c r="B22" s="94"/>
-      <c r="C22" s="94"/>
+      <c r="A22" s="75"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="56" t="s">
         <v>42</v>
       </c>
@@ -8211,9 +8249,9 @@
       <c r="P22" s="59"/>
     </row>
     <row r="23" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="93"/>
-      <c r="B23" s="94"/>
-      <c r="C23" s="84"/>
+      <c r="A23" s="75"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="79"/>
       <c r="D23" s="55" t="s">
         <v>43</v>
       </c>
@@ -8259,9 +8297,9 @@
       <c r="P23" s="59"/>
     </row>
     <row r="24" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="93"/>
-      <c r="B24" s="94"/>
-      <c r="C24" s="82" t="s">
+      <c r="A24" s="75"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="77" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="56" t="s">
@@ -8311,9 +8349,9 @@
       </c>
     </row>
     <row r="25" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="93"/>
-      <c r="B25" s="94"/>
-      <c r="C25" s="94"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="78"/>
       <c r="D25" s="55" t="s">
         <v>42</v>
       </c>
@@ -8355,9 +8393,9 @@
       <c r="P25" s="59"/>
     </row>
     <row r="26" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="93"/>
-      <c r="B26" s="94"/>
-      <c r="C26" s="84"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="79"/>
       <c r="D26" s="56" t="s">
         <v>43</v>
       </c>
@@ -8403,9 +8441,9 @@
       <c r="P26" s="59"/>
     </row>
     <row r="27" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="93"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="82" t="s">
+      <c r="A27" s="75"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="77" t="s">
         <v>114</v>
       </c>
       <c r="D27" s="55" t="s">
@@ -8453,9 +8491,9 @@
       </c>
     </row>
     <row r="28" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="93"/>
-      <c r="B28" s="94"/>
-      <c r="C28" s="94"/>
+      <c r="A28" s="75"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
       <c r="D28" s="56" t="s">
         <v>42</v>
       </c>
@@ -8500,9 +8538,9 @@
       </c>
     </row>
     <row r="29" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="81"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
+      <c r="A29" s="76"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="79"/>
       <c r="D29" s="55" t="s">
         <v>43</v>
       </c>
@@ -8548,13 +8586,13 @@
       <c r="P29" s="59"/>
     </row>
     <row r="30" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="76" t="s">
+      <c r="B30" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="76" t="s">
+      <c r="C30" s="83" t="s">
         <v>44</v>
       </c>
       <c r="D30" s="67" t="s">
@@ -8571,14 +8609,14 @@
         <v>149</v>
       </c>
       <c r="H30" s="66">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="I30" s="66">
-        <v>955</v>
+        <v>678</v>
       </c>
       <c r="J30" s="65">
         <f t="shared" si="2"/>
-        <v>1101</v>
+        <v>784</v>
       </c>
       <c r="K30" s="67">
         <v>0.25</v>
@@ -8592,7 +8630,7 @@
       </c>
       <c r="N30" s="60">
         <f t="shared" si="0"/>
-        <v>0.13260672116257946</v>
+        <v>0.13520408163265307</v>
       </c>
       <c r="O30" s="70">
         <f>G30/G31</f>
@@ -8603,9 +8641,9 @@
       </c>
     </row>
     <row r="31" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="74"/>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
+      <c r="A31" s="81"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="84"/>
       <c r="D31" s="68" t="s">
         <v>42</v>
       </c>
@@ -8620,14 +8658,14 @@
         <v>46</v>
       </c>
       <c r="H31" s="65">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="I31" s="65">
-        <v>299</v>
+        <v>213</v>
       </c>
       <c r="J31" s="65">
         <f t="shared" si="2"/>
-        <v>341</v>
+        <v>242</v>
       </c>
       <c r="K31" s="68">
         <v>0.17</v>
@@ -8641,15 +8679,15 @@
       </c>
       <c r="N31" s="60">
         <f t="shared" si="0"/>
-        <v>0.12316715542521994</v>
+        <v>0.11983471074380166</v>
       </c>
       <c r="O31" s="70"/>
       <c r="P31" s="70"/>
     </row>
     <row r="32" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="75"/>
-      <c r="B32" s="78"/>
-      <c r="C32" s="78"/>
+      <c r="A32" s="82"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="85"/>
       <c r="D32" s="67" t="s">
         <v>43</v>
       </c>
@@ -8667,15 +8705,15 @@
       </c>
       <c r="H32" s="66">
         <f>H31+H30</f>
-        <v>188</v>
+        <v>135</v>
       </c>
       <c r="I32" s="66">
         <f>I31+I30</f>
-        <v>1254</v>
+        <v>891</v>
       </c>
       <c r="J32" s="65">
         <f t="shared" si="2"/>
-        <v>1442</v>
+        <v>1026</v>
       </c>
       <c r="K32" s="67">
         <v>0.23</v>
@@ -8689,19 +8727,19 @@
       </c>
       <c r="N32" s="60">
         <f t="shared" si="0"/>
-        <v>0.13037447988904299</v>
+        <v>0.13157894736842105</v>
       </c>
       <c r="O32" s="70"/>
       <c r="P32" s="70"/>
     </row>
     <row r="33" spans="1:16" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="73" t="s">
+      <c r="A33" s="80" t="s">
         <v>117</v>
       </c>
-      <c r="B33" s="76" t="s">
+      <c r="B33" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="76" t="s">
+      <c r="C33" s="83" t="s">
         <v>40</v>
       </c>
       <c r="D33" s="68" t="s">
@@ -8747,9 +8785,9 @@
       </c>
     </row>
     <row r="34" spans="1:16" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="74"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
+      <c r="A34" s="81"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="84"/>
       <c r="D34" s="67" t="s">
         <v>42</v>
       </c>
@@ -8778,9 +8816,8 @@
       <c r="L34" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="M34" s="63">
-        <f t="shared" si="3"/>
-        <v>4.3478260869565216E-2</v>
+      <c r="M34" s="63" t="s">
+        <v>52</v>
       </c>
       <c r="N34" s="60" t="s">
         <v>52</v>
@@ -8789,9 +8826,9 @@
       <c r="P34" s="70"/>
     </row>
     <row r="35" spans="1:16" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="75"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="85"/>
       <c r="D35" s="68" t="s">
         <v>43</v>
       </c>
@@ -8833,13 +8870,13 @@
       <c r="P35" s="70"/>
     </row>
     <row r="36" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="79" t="s">
+      <c r="A36" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="82" t="s">
+      <c r="B36" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="82" t="s">
+      <c r="C36" s="77" t="s">
         <v>40</v>
       </c>
       <c r="D36" s="56" t="s">
@@ -8875,9 +8912,8 @@
         <f t="shared" si="3"/>
         <v>0.10457516339869281</v>
       </c>
-      <c r="N36" s="60">
-        <f t="shared" si="0"/>
-        <v>0.10810810810810811</v>
+      <c r="N36" s="60" t="s">
+        <v>52</v>
       </c>
       <c r="O36" s="59">
         <v>1.86585366</v>
@@ -8887,9 +8923,9 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="93"/>
-      <c r="B37" s="94"/>
-      <c r="C37" s="94"/>
+      <c r="A37" s="75"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="78"/>
       <c r="D37" s="55" t="s">
         <v>42</v>
       </c>
@@ -8923,17 +8959,16 @@
         <f t="shared" si="3"/>
         <v>0.14634146341463414</v>
       </c>
-      <c r="N37" s="60">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
+      <c r="N37" s="60" t="s">
+        <v>52</v>
       </c>
       <c r="O37" s="59"/>
       <c r="P37" s="59"/>
     </row>
     <row r="38" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="81"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="84"/>
+      <c r="A38" s="76"/>
+      <c r="B38" s="79"/>
+      <c r="C38" s="79"/>
       <c r="D38" s="56" t="s">
         <v>43</v>
       </c>
@@ -8979,13 +9014,13 @@
       <c r="P38" s="59"/>
     </row>
     <row r="39" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="79" t="s">
+      <c r="A39" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="82" t="s">
+      <c r="B39" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="82" t="s">
+      <c r="C39" s="77" t="s">
         <v>40</v>
       </c>
       <c r="D39" s="55" t="s">
@@ -9001,15 +9036,15 @@
         <f t="shared" si="1"/>
         <v>205</v>
       </c>
-      <c r="H39" s="65">
-        <v>146</v>
-      </c>
-      <c r="I39" s="65">
-        <v>955</v>
+      <c r="H39" s="66">
+        <v>106</v>
+      </c>
+      <c r="I39" s="66">
+        <v>678</v>
       </c>
       <c r="J39" s="65">
         <f t="shared" si="2"/>
-        <v>1101</v>
+        <v>784</v>
       </c>
       <c r="K39" s="55">
         <v>0.12</v>
@@ -9023,7 +9058,7 @@
       </c>
       <c r="N39" s="60">
         <f t="shared" si="0"/>
-        <v>0.13260672116257946</v>
+        <v>0.13520408163265307</v>
       </c>
       <c r="O39" s="70">
         <f>G39/G40</f>
@@ -9034,9 +9069,9 @@
       </c>
     </row>
     <row r="40" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="93"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="94"/>
+      <c r="A40" s="75"/>
+      <c r="B40" s="78"/>
+      <c r="C40" s="78"/>
       <c r="D40" s="56" t="s">
         <v>42</v>
       </c>
@@ -9051,14 +9086,14 @@
         <v>97</v>
       </c>
       <c r="H40" s="66">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I40" s="66">
-        <v>471</v>
+        <v>334</v>
       </c>
       <c r="J40" s="65">
         <f t="shared" si="2"/>
-        <v>522</v>
+        <v>372</v>
       </c>
       <c r="K40" s="56">
         <v>0.16</v>
@@ -9071,16 +9106,16 @@
         <v>0.16494845360824742</v>
       </c>
       <c r="N40" s="60">
-        <f t="shared" si="0"/>
-        <v>9.7701149425287362E-2</v>
+        <f>H40/J40</f>
+        <v>0.10215053763440861</v>
       </c>
       <c r="O40" s="59"/>
       <c r="P40" s="59"/>
     </row>
     <row r="41" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="81"/>
-      <c r="B41" s="84"/>
-      <c r="C41" s="84"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="79"/>
+      <c r="C41" s="79"/>
       <c r="D41" s="55" t="s">
         <v>43</v>
       </c>
@@ -9098,15 +9133,15 @@
       </c>
       <c r="H41" s="66">
         <f>H40+H39</f>
-        <v>197</v>
+        <v>144</v>
       </c>
       <c r="I41" s="66">
         <f>I40+I39</f>
-        <v>1426</v>
+        <v>1012</v>
       </c>
       <c r="J41" s="65">
-        <f t="shared" si="2"/>
-        <v>1623</v>
+        <f>H41+I41</f>
+        <v>1156</v>
       </c>
       <c r="K41" s="55">
         <v>0.13</v>
@@ -9120,19 +9155,19 @@
       </c>
       <c r="N41" s="60">
         <f t="shared" ref="N41:N48" si="11">H41/J41</f>
-        <v>0.12138016019716574</v>
+        <v>0.1245674740484429</v>
       </c>
       <c r="O41" s="59"/>
       <c r="P41" s="59"/>
     </row>
     <row r="42" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="79" t="s">
+      <c r="A42" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="82" t="s">
+      <c r="B42" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="82" t="s">
+      <c r="C42" s="77" t="s">
         <v>40</v>
       </c>
       <c r="D42" s="56" t="s">
@@ -9178,9 +9213,9 @@
       </c>
     </row>
     <row r="43" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="93"/>
-      <c r="B43" s="94"/>
-      <c r="C43" s="94"/>
+      <c r="A43" s="75"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="78"/>
       <c r="D43" s="55" t="s">
         <v>42</v>
       </c>
@@ -9216,9 +9251,9 @@
       <c r="P43" s="59"/>
     </row>
     <row r="44" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="93"/>
-      <c r="B44" s="94"/>
-      <c r="C44" s="84"/>
+      <c r="A44" s="75"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="79"/>
       <c r="D44" s="56" t="s">
         <v>43</v>
       </c>
@@ -9260,9 +9295,9 @@
       <c r="P44" s="59"/>
     </row>
     <row r="45" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="93"/>
-      <c r="B45" s="94"/>
-      <c r="C45" s="82" t="s">
+      <c r="A45" s="75"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="77" t="s">
         <v>44</v>
       </c>
       <c r="D45" s="55" t="s">
@@ -9308,9 +9343,9 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="93"/>
-      <c r="B46" s="94"/>
-      <c r="C46" s="94"/>
+      <c r="A46" s="75"/>
+      <c r="B46" s="78"/>
+      <c r="C46" s="78"/>
       <c r="D46" s="56" t="s">
         <v>42</v>
       </c>
@@ -9346,9 +9381,9 @@
       <c r="P46" s="59"/>
     </row>
     <row r="47" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="93"/>
-      <c r="B47" s="94"/>
-      <c r="C47" s="84"/>
+      <c r="A47" s="75"/>
+      <c r="B47" s="78"/>
+      <c r="C47" s="79"/>
       <c r="D47" s="55" t="s">
         <v>43</v>
       </c>
@@ -9390,9 +9425,9 @@
       <c r="P47" s="59"/>
     </row>
     <row r="48" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="93"/>
-      <c r="B48" s="94"/>
-      <c r="C48" s="82" t="s">
+      <c r="A48" s="75"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="77" t="s">
         <v>114</v>
       </c>
       <c r="D48" s="56" t="s">
@@ -9438,9 +9473,9 @@
       </c>
     </row>
     <row r="49" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="93"/>
-      <c r="B49" s="94"/>
-      <c r="C49" s="94"/>
+      <c r="A49" s="75"/>
+      <c r="B49" s="78"/>
+      <c r="C49" s="78"/>
       <c r="D49" s="55" t="s">
         <v>42</v>
       </c>
@@ -9476,9 +9511,9 @@
       <c r="P49" s="59"/>
     </row>
     <row r="50" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="81"/>
-      <c r="B50" s="84"/>
-      <c r="C50" s="84"/>
+      <c r="A50" s="76"/>
+      <c r="B50" s="79"/>
+      <c r="C50" s="79"/>
       <c r="D50" s="56" t="s">
         <v>43</v>
       </c>
@@ -9574,8 +9609,13 @@
         <v>1478</v>
       </c>
       <c r="H53" s="59"/>
-      <c r="I53" s="59"/>
-      <c r="J53" s="59"/>
+      <c r="I53" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="J53" s="59">
+        <f>G53-G17-G35</f>
+        <v>967</v>
+      </c>
       <c r="K53" s="59"/>
       <c r="L53" s="59"/>
       <c r="M53" s="59"/>
@@ -9591,7 +9631,7 @@
       </c>
       <c r="D54" s="59">
         <f>SUM(J11,J14,J17,J20,J29,J38,J50)</f>
-        <v>5120</v>
+        <v>4564</v>
       </c>
       <c r="E54" s="59"/>
       <c r="F54" s="59" t="s">
@@ -9617,7 +9657,7 @@
       </c>
       <c r="D55">
         <f>D54+D53</f>
-        <v>7582</v>
+        <v>7026</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
@@ -9626,7 +9666,7 @@
       </c>
       <c r="D56">
         <f>D55-G17-J17-G35</f>
-        <v>6021</v>
+        <v>5465</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
@@ -9638,15 +9678,33 @@
         <v>2033</v>
       </c>
     </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C58" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58">
+        <f>D54-J17</f>
+        <v>3514</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C59" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59">
+        <f>D57+D58</f>
+        <v>5547</v>
+      </c>
+    </row>
     <row r="62" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:16" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="85" t="s">
+      <c r="A63" s="87" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="88" t="s">
+      <c r="B63" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="88" t="s">
+      <c r="C63" s="90" t="s">
         <v>40</v>
       </c>
       <c r="D63" s="65" t="s">
@@ -9693,9 +9751,9 @@
       </c>
     </row>
     <row r="64" spans="1:16" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="86"/>
-      <c r="B64" s="89"/>
-      <c r="C64" s="89"/>
+      <c r="A64" s="88"/>
+      <c r="B64" s="91"/>
+      <c r="C64" s="91"/>
       <c r="D64" s="66" t="s">
         <v>42</v>
       </c>
@@ -9740,9 +9798,9 @@
       </c>
     </row>
     <row r="65" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="86"/>
-      <c r="B65" s="89"/>
-      <c r="C65" s="90"/>
+      <c r="A65" s="88"/>
+      <c r="B65" s="91"/>
+      <c r="C65" s="92"/>
       <c r="D65" s="65" t="s">
         <v>43</v>
       </c>
@@ -9785,9 +9843,9 @@
       <c r="P65" s="64"/>
     </row>
     <row r="66" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="86"/>
-      <c r="B66" s="89"/>
-      <c r="C66" s="88" t="s">
+      <c r="A66" s="88"/>
+      <c r="B66" s="91"/>
+      <c r="C66" s="90" t="s">
         <v>44</v>
       </c>
       <c r="D66" s="66" t="s">
@@ -9834,9 +9892,9 @@
       </c>
     </row>
     <row r="67" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="86"/>
-      <c r="B67" s="89"/>
-      <c r="C67" s="89"/>
+      <c r="A67" s="88"/>
+      <c r="B67" s="91"/>
+      <c r="C67" s="91"/>
       <c r="D67" s="65" t="s">
         <v>42</v>
       </c>
@@ -9881,9 +9939,9 @@
       </c>
     </row>
     <row r="68" spans="1:17" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="86"/>
-      <c r="B68" s="89"/>
-      <c r="C68" s="90"/>
+      <c r="A68" s="88"/>
+      <c r="B68" s="91"/>
+      <c r="C68" s="92"/>
       <c r="D68" s="66" t="s">
         <v>43</v>
       </c>
@@ -9924,9 +9982,9 @@
       <c r="P68" s="64"/>
     </row>
     <row r="69" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="86"/>
-      <c r="B69" s="89"/>
-      <c r="C69" s="88" t="s">
+      <c r="A69" s="88"/>
+      <c r="B69" s="91"/>
+      <c r="C69" s="90" t="s">
         <v>114</v>
       </c>
       <c r="D69" s="65" t="s">
@@ -9978,9 +10036,9 @@
       </c>
     </row>
     <row r="70" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="86"/>
-      <c r="B70" s="89"/>
-      <c r="C70" s="89"/>
+      <c r="A70" s="88"/>
+      <c r="B70" s="91"/>
+      <c r="C70" s="91"/>
       <c r="D70" s="66" t="s">
         <v>42</v>
       </c>
@@ -10021,9 +10079,9 @@
       <c r="P70" s="64"/>
     </row>
     <row r="71" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="87"/>
-      <c r="B71" s="90"/>
-      <c r="C71" s="90"/>
+      <c r="A71" s="89"/>
+      <c r="B71" s="92"/>
+      <c r="C71" s="92"/>
       <c r="D71" s="65" t="s">
         <v>43</v>
       </c>
@@ -10067,13 +10125,13 @@
       <c r="P71" s="64"/>
     </row>
     <row r="72" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="73" t="s">
+      <c r="A72" s="80" t="s">
         <v>134</v>
       </c>
-      <c r="B72" s="76" t="s">
+      <c r="B72" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="C72" s="76" t="s">
+      <c r="C72" s="83" t="s">
         <v>44</v>
       </c>
       <c r="D72" s="67" t="s">
@@ -10120,9 +10178,9 @@
       </c>
     </row>
     <row r="73" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="74"/>
-      <c r="B73" s="77"/>
-      <c r="C73" s="77"/>
+      <c r="A73" s="81"/>
+      <c r="B73" s="84"/>
+      <c r="C73" s="84"/>
       <c r="D73" s="71" t="s">
         <v>42</v>
       </c>
@@ -10163,9 +10221,9 @@
       <c r="P73" s="70"/>
     </row>
     <row r="74" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="75"/>
-      <c r="B74" s="78"/>
-      <c r="C74" s="78"/>
+      <c r="A74" s="82"/>
+      <c r="B74" s="85"/>
+      <c r="C74" s="85"/>
       <c r="D74" s="67" t="s">
         <v>43</v>
       </c>
@@ -10206,13 +10264,13 @@
       <c r="P74" s="70"/>
     </row>
     <row r="75" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="79" t="s">
+      <c r="A75" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="82" t="s">
+      <c r="B75" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C75" s="82" t="s">
+      <c r="C75" s="77" t="s">
         <v>40</v>
       </c>
       <c r="D75" s="58" t="s">
@@ -10259,9 +10317,9 @@
       </c>
     </row>
     <row r="76" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="80"/>
-      <c r="B76" s="83"/>
-      <c r="C76" s="83"/>
+      <c r="A76" s="94"/>
+      <c r="B76" s="95"/>
+      <c r="C76" s="95"/>
       <c r="D76" s="56" t="s">
         <v>42</v>
       </c>
@@ -10302,9 +10360,9 @@
       <c r="P76" s="59"/>
     </row>
     <row r="77" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="81"/>
-      <c r="B77" s="84"/>
-      <c r="C77" s="84"/>
+      <c r="A77" s="76"/>
+      <c r="B77" s="79"/>
+      <c r="C77" s="79"/>
       <c r="D77" s="58" t="s">
         <v>43</v>
       </c>
@@ -10344,33 +10402,133 @@
       <c r="O77" s="59"/>
       <c r="P77" s="59"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
+    <row r="81" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="100" t="s">
+        <v>135</v>
+      </c>
+      <c r="B81" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C81" s="98">
+        <v>146</v>
+      </c>
+      <c r="D81" s="98">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="100"/>
+      <c r="B82" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C82" s="99">
+        <v>88</v>
+      </c>
+      <c r="D82" s="99">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="100"/>
+      <c r="B83" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="C83" s="98">
+        <v>234</v>
+      </c>
+      <c r="D83" s="98">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="100" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84" s="66">
+        <v>146</v>
+      </c>
+      <c r="D84" s="66">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="100"/>
+      <c r="B85" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" s="72">
+        <v>42</v>
+      </c>
+      <c r="D85" s="72">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="100"/>
+      <c r="B86" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="C86" s="66">
+        <f>C85+C84</f>
+        <v>188</v>
+      </c>
+      <c r="D86" s="66">
+        <f>D85+D84</f>
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C87" s="72">
+        <v>146</v>
+      </c>
+      <c r="D87" s="72">
+        <v>955</v>
+      </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
+    <row r="88" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="101"/>
+      <c r="B88" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C88" s="66">
+        <v>51</v>
+      </c>
+      <c r="D88" s="66">
+        <v>471</v>
+      </c>
       <c r="E88" s="4"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
+    <row r="89" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="101"/>
+      <c r="B89" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="C89" s="66">
+        <f>C88+C87</f>
+        <v>197</v>
+      </c>
+      <c r="D89" s="66">
+        <f>D88+D87</f>
+        <v>1426</v>
+      </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -10469,38 +10627,21 @@
       <c r="J97" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="A42:A50"/>
-    <mergeCell ref="B42:B50"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="B21:B29"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
+  <mergeCells count="57">
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="A63:A71"/>
+    <mergeCell ref="B63:B71"/>
+    <mergeCell ref="C63:C65"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="C69:C71"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="B3:B11"/>
@@ -10513,17 +10654,37 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A63:A71"/>
-    <mergeCell ref="B63:B71"/>
-    <mergeCell ref="C63:C65"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="A42:A50"/>
+    <mergeCell ref="B42:B50"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10615,11 +10776,11 @@
       </c>
       <c r="D4" s="5">
         <f>Check_16052021!$H$11</f>
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="E4" s="5">
         <f>Check_16052021!$J$11</f>
-        <v>1931</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -10676,11 +10837,11 @@
       </c>
       <c r="D7" s="5">
         <f>Check_16052021!H32</f>
-        <v>188</v>
+        <v>135</v>
       </c>
       <c r="E7" s="5">
         <f>Check_16052021!J32</f>
-        <v>1442</v>
+        <v>1026</v>
       </c>
     </row>
   </sheetData>
@@ -10776,11 +10937,11 @@
       </c>
       <c r="D4" s="5">
         <f>Check_16052021!$H$10</f>
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5">
         <f>Check_16052021!$J$10</f>
-        <v>830</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -10818,11 +10979,11 @@
       </c>
       <c r="D6" s="5">
         <f>Check_16052021!$H$31</f>
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E6" s="5">
         <f>Check_16052021!$J$31</f>
-        <v>341</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -10913,11 +11074,11 @@
       </c>
       <c r="D4" s="5">
         <f>Check_16052021!$H$9</f>
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="E4" s="5">
         <f>Check_16052021!$J$9</f>
-        <v>1101</v>
+        <v>784</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -10955,11 +11116,11 @@
       </c>
       <c r="D6" s="5">
         <f>Check_16052021!$H$30</f>
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="E6" s="5">
         <f>Check_16052021!$J$30</f>
-        <v>1101</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>
@@ -11006,11 +11167,11 @@
       </c>
       <c r="D2" s="5">
         <f>Check_16052021!$H$41</f>
-        <v>197</v>
+        <v>144</v>
       </c>
       <c r="E2" s="5">
         <f>Check_16052021!$J$41</f>
-        <v>1623</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -11066,11 +11227,11 @@
       </c>
       <c r="D5" s="5">
         <f>Check_16052021!$H$11</f>
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="E5" s="5">
         <f>Check_16052021!$J$11</f>
-        <v>1931</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updating with single meta-analysis and moderators
</commit_message>
<xml_diff>
--- a/genlang_all_cohorts_updated.xlsx
+++ b/genlang_all_cohorts_updated.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippoabbondanza/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/sp58_st-andrews_ac_uk/Documents/gen_lang_hand_meta/GenLang_hand_preference_meta_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FF6E20-8800-5445-A236-C1846F152D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{E2FF6E20-8800-5445-A236-C1846F152D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EF8F9A3-3DC1-1E41-80C9-5A79B8ABD15A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{A6332151-AACC-E14E-B3DF-3D4980E70093}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A6332151-AACC-E14E-B3DF-3D4980E70093}"/>
   </bookViews>
   <sheets>
-    <sheet name="Combined2" sheetId="12" r:id="rId1"/>
-    <sheet name="Combined-Female2" sheetId="14" r:id="rId2"/>
-    <sheet name="Combined-Male2" sheetId="13" r:id="rId3"/>
-    <sheet name="All data" sheetId="23" r:id="rId4"/>
-    <sheet name="SLI-All" sheetId="1" r:id="rId5"/>
-    <sheet name="SLI-Female" sheetId="5" r:id="rId6"/>
-    <sheet name="SLI-Male" sheetId="6" r:id="rId7"/>
-    <sheet name="RD-All" sheetId="3" r:id="rId8"/>
-    <sheet name="RD-Female" sheetId="10" r:id="rId9"/>
-    <sheet name="RD-Male" sheetId="9" r:id="rId10"/>
+    <sheet name="sexmatch_strict_all_split" sheetId="24" r:id="rId1"/>
+    <sheet name="sexmatch_strict_all_split_0s" sheetId="25" r:id="rId2"/>
+    <sheet name="Combined2" sheetId="12" r:id="rId3"/>
+    <sheet name="Combined-Female2" sheetId="14" r:id="rId4"/>
+    <sheet name="Combined-Male2" sheetId="13" r:id="rId5"/>
+    <sheet name="All data" sheetId="23" r:id="rId6"/>
+    <sheet name="SLI-All" sheetId="1" r:id="rId7"/>
+    <sheet name="SLI-Female" sheetId="5" r:id="rId8"/>
+    <sheet name="SLI-Male" sheetId="6" r:id="rId9"/>
+    <sheet name="RD-All" sheetId="3" r:id="rId10"/>
+    <sheet name="RD-Female" sheetId="10" r:id="rId11"/>
+    <sheet name="RD-Male" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="77">
   <si>
     <t xml:space="preserve">TD Left-Handers </t>
   </si>
@@ -285,6 +287,42 @@
   </si>
   <si>
     <t>Tot Case + control (no NTR&lt;…)</t>
+  </si>
+  <si>
+    <t>cohort_name</t>
+  </si>
+  <si>
+    <t>cohort_type</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>cases_NRH</t>
+  </si>
+  <si>
+    <t>cases_RH</t>
+  </si>
+  <si>
+    <t>controls_NRH</t>
+  </si>
+  <si>
+    <t>controls_RH</t>
+  </si>
+  <si>
+    <t>total_cases</t>
+  </si>
+  <si>
+    <t>total_controls</t>
+  </si>
+  <si>
+    <t>NTR cohort</t>
+  </si>
+  <si>
+    <t>Multicenter Study Marburg/Würzburg cohort</t>
   </si>
 </sst>
 </file>
@@ -438,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -506,13 +544,49 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -542,28 +616,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -879,6 +944,2186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFDAA36-5674-0F4C-9112-EA4C27F6C29D}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="31">
+        <v>27</v>
+      </c>
+      <c r="F2" s="31">
+        <v>198</v>
+      </c>
+      <c r="G2" s="31">
+        <v>51</v>
+      </c>
+      <c r="H2" s="31">
+        <v>272</v>
+      </c>
+      <c r="I2" s="31">
+        <v>225</v>
+      </c>
+      <c r="J2" s="31">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="32">
+        <v>12</v>
+      </c>
+      <c r="F3" s="32">
+        <v>121</v>
+      </c>
+      <c r="G3" s="32">
+        <v>15</v>
+      </c>
+      <c r="H3" s="32">
+        <v>176</v>
+      </c>
+      <c r="I3" s="31">
+        <v>133</v>
+      </c>
+      <c r="J3" s="31">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="32">
+        <v>17</v>
+      </c>
+      <c r="F4" s="32">
+        <v>134</v>
+      </c>
+      <c r="G4" s="31">
+        <v>51</v>
+      </c>
+      <c r="H4" s="31">
+        <v>272</v>
+      </c>
+      <c r="I4" s="31">
+        <v>85</v>
+      </c>
+      <c r="J4" s="31">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="31">
+        <v>12</v>
+      </c>
+      <c r="F5" s="31">
+        <v>92</v>
+      </c>
+      <c r="G5" s="32">
+        <v>28</v>
+      </c>
+      <c r="H5" s="32">
+        <v>195</v>
+      </c>
+      <c r="I5" s="31">
+        <v>80</v>
+      </c>
+      <c r="J5" s="31">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="15">
+        <v>16</v>
+      </c>
+      <c r="F6" s="15">
+        <v>105</v>
+      </c>
+      <c r="G6" s="15">
+        <v>35</v>
+      </c>
+      <c r="H6" s="15">
+        <v>360</v>
+      </c>
+      <c r="I6" s="31">
+        <v>121</v>
+      </c>
+      <c r="J6" s="31">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="34">
+        <v>6</v>
+      </c>
+      <c r="F7" s="34">
+        <v>77</v>
+      </c>
+      <c r="G7" s="34">
+        <v>21</v>
+      </c>
+      <c r="H7" s="34">
+        <v>250</v>
+      </c>
+      <c r="I7" s="31">
+        <v>83</v>
+      </c>
+      <c r="J7" s="31">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="34">
+        <v>18</v>
+      </c>
+      <c r="F8" s="34">
+        <v>97</v>
+      </c>
+      <c r="G8" s="34">
+        <v>66</v>
+      </c>
+      <c r="H8" s="34">
+        <v>450</v>
+      </c>
+      <c r="I8" s="31">
+        <v>115</v>
+      </c>
+      <c r="J8" s="31">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="15">
+        <v>13</v>
+      </c>
+      <c r="F9" s="15">
+        <v>106</v>
+      </c>
+      <c r="G9" s="15">
+        <v>70</v>
+      </c>
+      <c r="H9" s="15">
+        <v>464</v>
+      </c>
+      <c r="I9" s="31">
+        <v>119</v>
+      </c>
+      <c r="J9" s="31">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="35">
+        <v>15</v>
+      </c>
+      <c r="F10" s="35">
+        <v>87</v>
+      </c>
+      <c r="G10" s="35">
+        <v>37</v>
+      </c>
+      <c r="H10" s="35">
+        <v>248</v>
+      </c>
+      <c r="I10" s="31">
+        <v>102</v>
+      </c>
+      <c r="J10" s="31">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="34">
+        <v>6</v>
+      </c>
+      <c r="F11" s="34">
+        <v>49</v>
+      </c>
+      <c r="G11" s="34">
+        <v>12</v>
+      </c>
+      <c r="H11" s="34">
+        <v>141</v>
+      </c>
+      <c r="I11" s="31">
+        <v>55</v>
+      </c>
+      <c r="J11" s="31">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="34">
+        <v>13</v>
+      </c>
+      <c r="F12" s="34">
+        <v>110</v>
+      </c>
+      <c r="G12" s="34">
+        <v>51</v>
+      </c>
+      <c r="H12" s="34">
+        <v>331</v>
+      </c>
+      <c r="I12" s="31">
+        <v>123</v>
+      </c>
+      <c r="J12" s="31">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="15">
+        <v>30</v>
+      </c>
+      <c r="F13" s="15">
+        <v>113</v>
+      </c>
+      <c r="G13" s="15">
+        <v>69</v>
+      </c>
+      <c r="H13" s="15">
+        <v>457</v>
+      </c>
+      <c r="I13" s="31">
+        <v>143</v>
+      </c>
+      <c r="J13" s="31">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="35">
+        <v>13</v>
+      </c>
+      <c r="F14" s="35">
+        <v>73</v>
+      </c>
+      <c r="G14" s="35">
+        <v>51</v>
+      </c>
+      <c r="H14" s="35">
+        <v>331</v>
+      </c>
+      <c r="I14" s="31">
+        <v>86</v>
+      </c>
+      <c r="J14" s="31">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="34">
+        <v>20</v>
+      </c>
+      <c r="F15" s="34">
+        <v>117</v>
+      </c>
+      <c r="G15" s="34">
+        <v>69</v>
+      </c>
+      <c r="H15" s="34">
+        <v>457</v>
+      </c>
+      <c r="I15" s="31">
+        <v>137</v>
+      </c>
+      <c r="J15" s="31">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="15">
+        <v>37</v>
+      </c>
+      <c r="F16" s="15">
+        <v>112</v>
+      </c>
+      <c r="G16" s="32">
+        <v>39</v>
+      </c>
+      <c r="H16" s="32">
+        <v>279</v>
+      </c>
+      <c r="I16" s="31">
+        <v>149</v>
+      </c>
+      <c r="J16" s="31">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="34">
+        <v>8</v>
+      </c>
+      <c r="F17" s="34">
+        <v>38</v>
+      </c>
+      <c r="G17" s="31">
+        <v>11</v>
+      </c>
+      <c r="H17" s="31">
+        <v>87</v>
+      </c>
+      <c r="I17" s="31">
+        <v>46</v>
+      </c>
+      <c r="J17" s="31">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="34">
+        <v>19</v>
+      </c>
+      <c r="F18" s="34">
+        <v>189</v>
+      </c>
+      <c r="G18" s="34">
+        <v>0</v>
+      </c>
+      <c r="H18" s="34">
+        <v>0</v>
+      </c>
+      <c r="I18" s="31">
+        <v>208</v>
+      </c>
+      <c r="J18" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0</v>
+      </c>
+      <c r="F19" s="15">
+        <v>66</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0</v>
+      </c>
+      <c r="I19" s="31">
+        <v>66</v>
+      </c>
+      <c r="J19" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="35">
+        <v>16</v>
+      </c>
+      <c r="F20" s="35">
+        <v>137</v>
+      </c>
+      <c r="G20" s="35">
+        <v>4</v>
+      </c>
+      <c r="H20" s="35">
+        <v>33</v>
+      </c>
+      <c r="I20" s="31">
+        <v>153</v>
+      </c>
+      <c r="J20" s="31">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="34">
+        <v>12</v>
+      </c>
+      <c r="F21" s="34">
+        <v>70</v>
+      </c>
+      <c r="G21" s="34">
+        <v>3</v>
+      </c>
+      <c r="H21" s="34">
+        <v>17</v>
+      </c>
+      <c r="I21" s="31">
+        <v>82</v>
+      </c>
+      <c r="J21" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="34">
+        <v>24</v>
+      </c>
+      <c r="F22" s="34">
+        <v>181</v>
+      </c>
+      <c r="G22" s="61">
+        <v>38</v>
+      </c>
+      <c r="H22" s="61">
+        <v>262</v>
+      </c>
+      <c r="I22" s="31">
+        <v>205</v>
+      </c>
+      <c r="J22" s="31">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="15">
+        <v>16</v>
+      </c>
+      <c r="F23" s="15">
+        <v>81</v>
+      </c>
+      <c r="G23" s="61">
+        <v>7</v>
+      </c>
+      <c r="H23" s="61">
+        <v>135</v>
+      </c>
+      <c r="I23" s="31">
+        <v>97</v>
+      </c>
+      <c r="J23" s="31">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="34">
+        <v>8</v>
+      </c>
+      <c r="F24" s="34">
+        <v>18</v>
+      </c>
+      <c r="G24" s="35">
+        <v>11</v>
+      </c>
+      <c r="H24" s="35">
+        <v>37</v>
+      </c>
+      <c r="I24" s="31">
+        <v>26</v>
+      </c>
+      <c r="J24" s="31">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="34">
+        <v>3</v>
+      </c>
+      <c r="F25" s="34">
+        <v>7</v>
+      </c>
+      <c r="G25" s="34">
+        <v>0</v>
+      </c>
+      <c r="H25" s="34">
+        <v>18</v>
+      </c>
+      <c r="I25" s="31">
+        <v>7</v>
+      </c>
+      <c r="J25" s="31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="34">
+        <v>8</v>
+      </c>
+      <c r="F26" s="34">
+        <v>18</v>
+      </c>
+      <c r="G26" s="35">
+        <v>11</v>
+      </c>
+      <c r="H26" s="35">
+        <v>37</v>
+      </c>
+      <c r="I26" s="31">
+        <v>9</v>
+      </c>
+      <c r="J26" s="31">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="34">
+        <v>1</v>
+      </c>
+      <c r="F27" s="34">
+        <v>12</v>
+      </c>
+      <c r="G27" s="34">
+        <v>2</v>
+      </c>
+      <c r="H27" s="34">
+        <v>29</v>
+      </c>
+      <c r="I27" s="31">
+        <v>7</v>
+      </c>
+      <c r="J27" s="31">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC87D760-B96E-3246-9702-6C0D2F3D090B}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>302</v>
+      </c>
+      <c r="D2" s="5">
+        <f>'All data'!$H$41</f>
+        <v>144</v>
+      </c>
+      <c r="E2" s="5">
+        <f>'All data'!$J$41</f>
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <f>28+70+137</f>
+        <v>235</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <f>7+33+17</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <f>223+43</f>
+        <v>266</v>
+      </c>
+      <c r="D4">
+        <f>70+50</f>
+        <v>120</v>
+      </c>
+      <c r="E4">
+        <f>526+382</f>
+        <v>908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5">
+        <f>'All data'!E5</f>
+        <v>16</v>
+      </c>
+      <c r="C5" s="5">
+        <f>'All data'!G5</f>
+        <v>114</v>
+      </c>
+      <c r="D5" s="5">
+        <f>'All data'!$H$11</f>
+        <v>169</v>
+      </c>
+      <c r="E5" s="5">
+        <f>'All data'!$J$11</f>
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <f>31+203</f>
+        <v>234</v>
+      </c>
+      <c r="D6">
+        <v>136</v>
+      </c>
+      <c r="E6">
+        <f>136+914</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <f>'All data'!E44</f>
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <f>'All data'!G44</f>
+        <v>50</v>
+      </c>
+      <c r="D7" s="9">
+        <f>'All data'!H44</f>
+        <v>14</v>
+      </c>
+      <c r="E7" s="9">
+        <f>'All data'!J44</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872AA266-2735-8C43-9155-1133034A0A26}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C2" t="e">
+        <f>#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D2" s="5">
+        <f>'All data'!$H$40</f>
+        <v>38</v>
+      </c>
+      <c r="E2" s="5">
+        <f>'All data'!$J$40</f>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C3" t="e">
+        <f>#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D3" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E3" t="e">
+        <f>#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5">
+        <f>'All data'!E4</f>
+        <v>10</v>
+      </c>
+      <c r="C4" s="5">
+        <f>'All data'!G4</f>
+        <v>60</v>
+      </c>
+      <c r="D4" s="5">
+        <f>'All data'!$H$10</f>
+        <v>63</v>
+      </c>
+      <c r="E4" s="5">
+        <f>'All data'!$J$10</f>
+        <v>591</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <f>13+106</f>
+        <v>119</v>
+      </c>
+      <c r="D5">
+        <v>70</v>
+      </c>
+      <c r="E5">
+        <f>70+464</f>
+        <v>534</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8282C54D-ECEF-5B4A-B2FE-0D87E182EEEB}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C2" t="e">
+        <f>#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D2" s="5">
+        <f>'All data'!$H$39</f>
+        <v>106</v>
+      </c>
+      <c r="E2" s="5">
+        <f>'All data'!$J$39</f>
+        <v>784</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C3" t="e">
+        <f>#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D3" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E3" t="e">
+        <f>#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5">
+        <f>'All data'!E3</f>
+        <v>6</v>
+      </c>
+      <c r="C4" s="5">
+        <f>'All data'!G3</f>
+        <v>54</v>
+      </c>
+      <c r="D4" s="5">
+        <f>'All data'!H3</f>
+        <v>106</v>
+      </c>
+      <c r="E4" s="5">
+        <f>'All data'!J3</f>
+        <v>784</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <f>18+97</f>
+        <v>115</v>
+      </c>
+      <c r="D5">
+        <v>66</v>
+      </c>
+      <c r="E5">
+        <f>66+450</f>
+        <v>516</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E80D89-0352-3447-97C9-D167DAAC1D84}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="31">
+        <v>27</v>
+      </c>
+      <c r="F2" s="31">
+        <v>198</v>
+      </c>
+      <c r="G2" s="31">
+        <v>51</v>
+      </c>
+      <c r="H2" s="31">
+        <v>272</v>
+      </c>
+      <c r="I2" s="31">
+        <v>225</v>
+      </c>
+      <c r="J2" s="31">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="32">
+        <v>12</v>
+      </c>
+      <c r="F3" s="32">
+        <v>121</v>
+      </c>
+      <c r="G3" s="32">
+        <v>15</v>
+      </c>
+      <c r="H3" s="32">
+        <v>176</v>
+      </c>
+      <c r="I3" s="31">
+        <v>133</v>
+      </c>
+      <c r="J3" s="31">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="32">
+        <v>17</v>
+      </c>
+      <c r="F4" s="32">
+        <v>134</v>
+      </c>
+      <c r="G4" s="31">
+        <v>51</v>
+      </c>
+      <c r="H4" s="31">
+        <v>272</v>
+      </c>
+      <c r="I4" s="31">
+        <v>85</v>
+      </c>
+      <c r="J4" s="31">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="31">
+        <v>12</v>
+      </c>
+      <c r="F5" s="31">
+        <v>92</v>
+      </c>
+      <c r="G5" s="32">
+        <v>28</v>
+      </c>
+      <c r="H5" s="32">
+        <v>195</v>
+      </c>
+      <c r="I5" s="31">
+        <v>80</v>
+      </c>
+      <c r="J5" s="31">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="15">
+        <v>16</v>
+      </c>
+      <c r="F6" s="15">
+        <v>105</v>
+      </c>
+      <c r="G6" s="15">
+        <v>35</v>
+      </c>
+      <c r="H6" s="15">
+        <v>360</v>
+      </c>
+      <c r="I6" s="31">
+        <v>121</v>
+      </c>
+      <c r="J6" s="31">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="34">
+        <v>6</v>
+      </c>
+      <c r="F7" s="34">
+        <v>77</v>
+      </c>
+      <c r="G7" s="34">
+        <v>21</v>
+      </c>
+      <c r="H7" s="34">
+        <v>250</v>
+      </c>
+      <c r="I7" s="31">
+        <v>83</v>
+      </c>
+      <c r="J7" s="31">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="34">
+        <v>18</v>
+      </c>
+      <c r="F8" s="34">
+        <v>97</v>
+      </c>
+      <c r="G8" s="34">
+        <v>66</v>
+      </c>
+      <c r="H8" s="34">
+        <v>450</v>
+      </c>
+      <c r="I8" s="31">
+        <v>115</v>
+      </c>
+      <c r="J8" s="31">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="15">
+        <v>13</v>
+      </c>
+      <c r="F9" s="15">
+        <v>106</v>
+      </c>
+      <c r="G9" s="15">
+        <v>70</v>
+      </c>
+      <c r="H9" s="15">
+        <v>464</v>
+      </c>
+      <c r="I9" s="31">
+        <v>119</v>
+      </c>
+      <c r="J9" s="31">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="35">
+        <v>15</v>
+      </c>
+      <c r="F10" s="35">
+        <v>87</v>
+      </c>
+      <c r="G10" s="35">
+        <v>37</v>
+      </c>
+      <c r="H10" s="35">
+        <v>248</v>
+      </c>
+      <c r="I10" s="31">
+        <v>102</v>
+      </c>
+      <c r="J10" s="31">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="34">
+        <v>6</v>
+      </c>
+      <c r="F11" s="34">
+        <v>49</v>
+      </c>
+      <c r="G11" s="34">
+        <v>12</v>
+      </c>
+      <c r="H11" s="34">
+        <v>141</v>
+      </c>
+      <c r="I11" s="31">
+        <v>55</v>
+      </c>
+      <c r="J11" s="31">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="34">
+        <v>13</v>
+      </c>
+      <c r="F12" s="34">
+        <v>110</v>
+      </c>
+      <c r="G12" s="34">
+        <v>51</v>
+      </c>
+      <c r="H12" s="34">
+        <v>331</v>
+      </c>
+      <c r="I12" s="31">
+        <v>123</v>
+      </c>
+      <c r="J12" s="31">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="15">
+        <v>30</v>
+      </c>
+      <c r="F13" s="15">
+        <v>113</v>
+      </c>
+      <c r="G13" s="15">
+        <v>69</v>
+      </c>
+      <c r="H13" s="15">
+        <v>457</v>
+      </c>
+      <c r="I13" s="31">
+        <v>143</v>
+      </c>
+      <c r="J13" s="31">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="35">
+        <v>13</v>
+      </c>
+      <c r="F14" s="35">
+        <v>73</v>
+      </c>
+      <c r="G14" s="35">
+        <v>51</v>
+      </c>
+      <c r="H14" s="35">
+        <v>331</v>
+      </c>
+      <c r="I14" s="31">
+        <v>86</v>
+      </c>
+      <c r="J14" s="31">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="34">
+        <v>20</v>
+      </c>
+      <c r="F15" s="34">
+        <v>117</v>
+      </c>
+      <c r="G15" s="34">
+        <v>69</v>
+      </c>
+      <c r="H15" s="34">
+        <v>457</v>
+      </c>
+      <c r="I15" s="31">
+        <v>137</v>
+      </c>
+      <c r="J15" s="31">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="15">
+        <v>37</v>
+      </c>
+      <c r="F16" s="15">
+        <v>112</v>
+      </c>
+      <c r="G16" s="32">
+        <v>39</v>
+      </c>
+      <c r="H16" s="32">
+        <v>279</v>
+      </c>
+      <c r="I16" s="31">
+        <v>149</v>
+      </c>
+      <c r="J16" s="31">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="34">
+        <v>8</v>
+      </c>
+      <c r="F17" s="34">
+        <v>38</v>
+      </c>
+      <c r="G17" s="31">
+        <v>11</v>
+      </c>
+      <c r="H17" s="31">
+        <v>87</v>
+      </c>
+      <c r="I17" s="31">
+        <v>46</v>
+      </c>
+      <c r="J17" s="31">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="34">
+        <v>19</v>
+      </c>
+      <c r="F18" s="34">
+        <v>189</v>
+      </c>
+      <c r="G18" s="34">
+        <v>0</v>
+      </c>
+      <c r="H18" s="34">
+        <v>0</v>
+      </c>
+      <c r="I18" s="31">
+        <v>208</v>
+      </c>
+      <c r="J18" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0</v>
+      </c>
+      <c r="F19" s="15">
+        <v>66</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0</v>
+      </c>
+      <c r="I19" s="31">
+        <v>66</v>
+      </c>
+      <c r="J19" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="35">
+        <v>16</v>
+      </c>
+      <c r="F20" s="35">
+        <v>137</v>
+      </c>
+      <c r="G20" s="35">
+        <v>0</v>
+      </c>
+      <c r="H20" s="35">
+        <v>33</v>
+      </c>
+      <c r="I20" s="31">
+        <v>153</v>
+      </c>
+      <c r="J20" s="31">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="34">
+        <v>12</v>
+      </c>
+      <c r="F21" s="34">
+        <v>70</v>
+      </c>
+      <c r="G21" s="34">
+        <v>0</v>
+      </c>
+      <c r="H21" s="34">
+        <v>17</v>
+      </c>
+      <c r="I21" s="31">
+        <v>82</v>
+      </c>
+      <c r="J21" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="34">
+        <v>24</v>
+      </c>
+      <c r="F22" s="34">
+        <v>181</v>
+      </c>
+      <c r="G22" s="61">
+        <v>38</v>
+      </c>
+      <c r="H22" s="61">
+        <v>262</v>
+      </c>
+      <c r="I22" s="31">
+        <v>205</v>
+      </c>
+      <c r="J22" s="31">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="15">
+        <v>16</v>
+      </c>
+      <c r="F23" s="15">
+        <v>81</v>
+      </c>
+      <c r="G23" s="61">
+        <v>7</v>
+      </c>
+      <c r="H23" s="61">
+        <v>135</v>
+      </c>
+      <c r="I23" s="31">
+        <v>97</v>
+      </c>
+      <c r="J23" s="31">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="34">
+        <v>8</v>
+      </c>
+      <c r="F24" s="34">
+        <v>18</v>
+      </c>
+      <c r="G24" s="35">
+        <v>11</v>
+      </c>
+      <c r="H24" s="35">
+        <v>37</v>
+      </c>
+      <c r="I24" s="31">
+        <v>26</v>
+      </c>
+      <c r="J24" s="31">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="34">
+        <v>0</v>
+      </c>
+      <c r="F25" s="34">
+        <v>7</v>
+      </c>
+      <c r="G25" s="34">
+        <v>0</v>
+      </c>
+      <c r="H25" s="34">
+        <v>18</v>
+      </c>
+      <c r="I25" s="31">
+        <v>7</v>
+      </c>
+      <c r="J25" s="31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="34">
+        <v>8</v>
+      </c>
+      <c r="F26" s="34">
+        <v>18</v>
+      </c>
+      <c r="G26" s="35">
+        <v>11</v>
+      </c>
+      <c r="H26" s="35">
+        <v>37</v>
+      </c>
+      <c r="I26" s="31">
+        <v>9</v>
+      </c>
+      <c r="J26" s="31">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="34">
+        <v>0</v>
+      </c>
+      <c r="F27" s="34">
+        <v>12</v>
+      </c>
+      <c r="G27" s="34">
+        <v>0</v>
+      </c>
+      <c r="H27" s="34">
+        <v>29</v>
+      </c>
+      <c r="I27" s="31">
+        <v>7</v>
+      </c>
+      <c r="J27" s="31">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DC49C6-505E-DC43-883F-74098BEBDD3C}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1133,121 +3378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8282C54D-ECEF-5B4A-B2FE-0D87E182EEEB}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C2" t="e">
-        <f>#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D2" s="5">
-        <f>'All data'!$H$39</f>
-        <v>106</v>
-      </c>
-      <c r="E2" s="5">
-        <f>'All data'!$J$39</f>
-        <v>784</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C3" t="e">
-        <f>#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D3" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E3" t="e">
-        <f>#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5">
-        <f>'All data'!E3</f>
-        <v>6</v>
-      </c>
-      <c r="C4" s="5">
-        <f>'All data'!G3</f>
-        <v>54</v>
-      </c>
-      <c r="D4" s="5">
-        <f>'All data'!H3</f>
-        <v>106</v>
-      </c>
-      <c r="E4" s="5">
-        <f>'All data'!J3</f>
-        <v>784</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <f>18+97</f>
-        <v>115</v>
-      </c>
-      <c r="D5">
-        <v>66</v>
-      </c>
-      <c r="E5">
-        <f>66+450</f>
-        <v>516</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8078E827-9226-664E-A5DC-9CAE983779B2}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -1443,7 +3574,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB91A93-20D8-5240-A569-93FEDF0E77E0}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -1640,11 +3771,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928079C8-A45F-5648-B92F-F547C22F48B1}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+    <sheetView zoomScale="92" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E57" sqref="E57:E60"/>
     </sheetView>
@@ -1657,42 +3788,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="52"/>
+      <c r="F1" s="46"/>
       <c r="G1" s="11"/>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="52"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="11"/>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="45"/>
+      <c r="L1" s="37"/>
       <c r="M1" s="18"/>
       <c r="N1" s="18"/>
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="16" t="s">
         <v>36</v>
       </c>
@@ -1731,13 +3862,13 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="41" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="21" t="s">
@@ -1785,9 +3916,9 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="25" t="s">
         <v>26</v>
       </c>
@@ -1829,9 +3960,9 @@
       <c r="P4" s="23"/>
     </row>
     <row r="5" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="21" t="s">
         <v>27</v>
       </c>
@@ -1875,9 +4006,9 @@
       <c r="P5" s="23"/>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="49" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="41" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="25" t="s">
@@ -1925,9 +4056,9 @@
       </c>
     </row>
     <row r="7" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="21" t="s">
         <v>26</v>
       </c>
@@ -1969,9 +4100,9 @@
       <c r="P7" s="23"/>
     </row>
     <row r="8" spans="1:17" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="51"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="25" t="s">
         <v>27</v>
       </c>
@@ -2015,9 +4146,9 @@
       <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="49" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="41" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="21" t="s">
@@ -2070,9 +4201,9 @@
       </c>
     </row>
     <row r="10" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="25" t="s">
         <v>26</v>
       </c>
@@ -2113,9 +4244,9 @@
       <c r="P10" s="23"/>
     </row>
     <row r="11" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="21" t="s">
         <v>27</v>
       </c>
@@ -2159,13 +4290,13 @@
       <c r="P11" s="23"/>
     </row>
     <row r="12" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="48" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -2213,9 +4344,9 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
@@ -2257,9 +4388,9 @@
       <c r="P13" s="18"/>
     </row>
     <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="15" t="s">
         <v>27</v>
       </c>
@@ -2303,13 +4434,13 @@
       <c r="P14" s="18"/>
     </row>
     <row r="15" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="54" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="27" t="s">
@@ -2357,9 +4488,9 @@
       </c>
     </row>
     <row r="16" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="26" t="s">
         <v>26</v>
       </c>
@@ -2401,9 +4532,9 @@
       <c r="P16" s="28"/>
     </row>
     <row r="17" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="27" t="s">
         <v>27</v>
       </c>
@@ -2449,13 +4580,13 @@
       <c r="P17" s="28"/>
     </row>
     <row r="18" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="48" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="15" t="s">
@@ -2503,9 +4634,9 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="14" t="s">
         <v>26</v>
       </c>
@@ -2547,9 +4678,9 @@
       <c r="P19" s="18"/>
     </row>
     <row r="20" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="15" t="s">
         <v>27</v>
       </c>
@@ -2595,13 +4726,13 @@
       <c r="P20" s="18"/>
     </row>
     <row r="21" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="48" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="14" t="s">
@@ -2649,9 +4780,9 @@
       </c>
     </row>
     <row r="22" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="15" t="s">
         <v>26</v>
       </c>
@@ -2693,9 +4824,9 @@
       <c r="P22" s="18"/>
     </row>
     <row r="23" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="38"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="14" t="s">
         <v>27</v>
       </c>
@@ -2741,9 +4872,9 @@
       <c r="P23" s="18"/>
     </row>
     <row r="24" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="36" t="s">
+      <c r="A24" s="47"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="48" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="15" t="s">
@@ -2793,9 +4924,9 @@
       </c>
     </row>
     <row r="25" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="14" t="s">
         <v>26</v>
       </c>
@@ -2837,9 +4968,9 @@
       <c r="P25" s="18"/>
     </row>
     <row r="26" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="15" t="s">
         <v>27</v>
       </c>
@@ -2885,9 +5016,9 @@
       <c r="P26" s="18"/>
     </row>
     <row r="27" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="36" t="s">
+      <c r="A27" s="47"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="48" t="s">
         <v>43</v>
       </c>
       <c r="D27" s="14" t="s">
@@ -2935,9 +5066,9 @@
       </c>
     </row>
     <row r="28" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="15" t="s">
         <v>26</v>
       </c>
@@ -2982,9 +5113,9 @@
       </c>
     </row>
     <row r="29" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="14" t="s">
         <v>27</v>
       </c>
@@ -3030,13 +5161,13 @@
       <c r="P29" s="18"/>
     </row>
     <row r="30" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="54" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="26" t="s">
@@ -3085,9 +5216,9 @@
       </c>
     </row>
     <row r="31" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
       <c r="D31" s="27" t="s">
         <v>26</v>
       </c>
@@ -3129,9 +5260,9 @@
       <c r="P31" s="28"/>
     </row>
     <row r="32" spans="1:17" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
       <c r="D32" s="26" t="s">
         <v>27</v>
       </c>
@@ -3177,13 +5308,13 @@
       <c r="P32" s="28"/>
     </row>
     <row r="33" spans="1:16" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="54" t="s">
         <v>24</v>
       </c>
       <c r="D33" s="27" t="s">
@@ -3229,9 +5360,9 @@
       </c>
     </row>
     <row r="34" spans="1:16" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="40"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
       <c r="D34" s="26" t="s">
         <v>26</v>
       </c>
@@ -3270,9 +5401,9 @@
       <c r="P34" s="28"/>
     </row>
     <row r="35" spans="1:16" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
       <c r="D35" s="27" t="s">
         <v>27</v>
       </c>
@@ -3314,13 +5445,13 @@
       <c r="P35" s="28"/>
     </row>
     <row r="36" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="48" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="15" t="s">
@@ -3367,9 +5498,9 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
       <c r="D37" s="14" t="s">
         <v>26</v>
       </c>
@@ -3410,9 +5541,9 @@
       <c r="P37" s="18"/>
     </row>
     <row r="38" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
+      <c r="A38" s="45"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
       <c r="D38" s="15" t="s">
         <v>27</v>
       </c>
@@ -3458,13 +5589,13 @@
       <c r="P38" s="18"/>
     </row>
     <row r="39" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="48" t="s">
         <v>24</v>
       </c>
       <c r="D39" s="14" t="s">
@@ -3513,9 +5644,9 @@
       </c>
     </row>
     <row r="40" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
       <c r="D40" s="15" t="s">
         <v>26</v>
       </c>
@@ -3557,9 +5688,9 @@
       <c r="P40" s="18"/>
     </row>
     <row r="41" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
+      <c r="A41" s="45"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="14" t="s">
         <v>27</v>
       </c>
@@ -3605,13 +5736,13 @@
       <c r="P41" s="18"/>
     </row>
     <row r="42" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="48" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="15" t="s">
@@ -3657,9 +5788,9 @@
       </c>
     </row>
     <row r="43" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
+      <c r="A43" s="47"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="14" t="s">
         <v>26</v>
       </c>
@@ -3695,9 +5826,9 @@
       <c r="P43" s="18"/>
     </row>
     <row r="44" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="38"/>
+      <c r="A44" s="47"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="15" t="s">
         <v>27</v>
       </c>
@@ -3739,9 +5870,9 @@
       <c r="P44" s="18"/>
     </row>
     <row r="45" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="34"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="36" t="s">
+      <c r="A45" s="47"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="48" t="s">
         <v>28</v>
       </c>
       <c r="D45" s="14" t="s">
@@ -3787,9 +5918,9 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
+      <c r="A46" s="47"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="15" t="s">
         <v>26</v>
       </c>
@@ -3825,9 +5956,9 @@
       <c r="P46" s="18"/>
     </row>
     <row r="47" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="38"/>
+      <c r="A47" s="47"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="50"/>
       <c r="D47" s="14" t="s">
         <v>27</v>
       </c>
@@ -3869,9 +6000,9 @@
       <c r="P47" s="18"/>
     </row>
     <row r="48" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="36" t="s">
+      <c r="A48" s="47"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="48" t="s">
         <v>43</v>
       </c>
       <c r="D48" s="15" t="s">
@@ -3917,9 +6048,9 @@
       </c>
     </row>
     <row r="49" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
+      <c r="A49" s="47"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
       <c r="D49" s="14" t="s">
         <v>26</v>
       </c>
@@ -3955,9 +6086,9 @@
       <c r="P49" s="18"/>
     </row>
     <row r="50" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
+      <c r="A50" s="45"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
       <c r="D50" s="15" t="s">
         <v>27</v>
       </c>
@@ -4142,6 +6273,37 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A42:A50"/>
+    <mergeCell ref="B42:B50"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="B3:B11"/>
@@ -4154,43 +6316,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="B21:B29"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A42:A50"/>
-    <mergeCell ref="B42:B50"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875C58A0-AE3B-164A-826D-BCBAEC3E436B}">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -4350,7 +6481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C273FEF-7270-914F-9008-FD5984BFD23F}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -4491,7 +6622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92E7F40-3DCB-9F42-8DBE-43E3A4FFD2E1}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -4626,312 +6757,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC87D760-B96E-3246-9702-6C0D2F3D090B}">
-  <dimension ref="A1:I32"/>
-  <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2">
-        <v>40</v>
-      </c>
-      <c r="C2">
-        <v>302</v>
-      </c>
-      <c r="D2" s="5">
-        <f>'All data'!$H$41</f>
-        <v>144</v>
-      </c>
-      <c r="E2" s="5">
-        <f>'All data'!$J$41</f>
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>28</v>
-      </c>
-      <c r="C3">
-        <f>28+70+137</f>
-        <v>235</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <f>7+33+17</f>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>43</v>
-      </c>
-      <c r="C4">
-        <f>223+43</f>
-        <v>266</v>
-      </c>
-      <c r="D4">
-        <f>70+50</f>
-        <v>120</v>
-      </c>
-      <c r="E4">
-        <f>526+382</f>
-        <v>908</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5">
-        <f>'All data'!E5</f>
-        <v>16</v>
-      </c>
-      <c r="C5" s="5">
-        <f>'All data'!G5</f>
-        <v>114</v>
-      </c>
-      <c r="D5" s="5">
-        <f>'All data'!$H$11</f>
-        <v>169</v>
-      </c>
-      <c r="E5" s="5">
-        <f>'All data'!$J$11</f>
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>31</v>
-      </c>
-      <c r="C6">
-        <f>31+203</f>
-        <v>234</v>
-      </c>
-      <c r="D6">
-        <v>136</v>
-      </c>
-      <c r="E6">
-        <f>136+914</f>
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <f>'All data'!E44</f>
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <f>'All data'!G44</f>
-        <v>50</v>
-      </c>
-      <c r="D7" s="9">
-        <f>'All data'!H44</f>
-        <v>14</v>
-      </c>
-      <c r="E7" s="9">
-        <f>'All data'!J44</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872AA266-2735-8C43-9155-1133034A0A26}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C2" t="e">
-        <f>#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D2" s="5">
-        <f>'All data'!$H$40</f>
-        <v>38</v>
-      </c>
-      <c r="E2" s="5">
-        <f>'All data'!$J$40</f>
-        <v>372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C3" t="e">
-        <f>#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D3" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E3" t="e">
-        <f>#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5">
-        <f>'All data'!E4</f>
-        <v>10</v>
-      </c>
-      <c r="C4" s="5">
-        <f>'All data'!G4</f>
-        <v>60</v>
-      </c>
-      <c r="D4" s="5">
-        <f>'All data'!$H$10</f>
-        <v>63</v>
-      </c>
-      <c r="E4" s="5">
-        <f>'All data'!$J$10</f>
-        <v>591</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <f>13+106</f>
-        <v>119</v>
-      </c>
-      <c r="D5">
-        <v>70</v>
-      </c>
-      <c r="E5">
-        <f>70+464</f>
-        <v>534</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding new revision with updated TEDS and meta-analysis
</commit_message>
<xml_diff>
--- a/genlang_all_cohorts_updated.xlsx
+++ b/genlang_all_cohorts_updated.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippoabbondanza/University of St Andrews/Silvia Paracchini - gen_lang_hand_meta/GenLang_hand_preference_meta_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippoabbondanza/Documents/PhD/GenLang_hand_preference_meta_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6D3491-1A0F-BD42-AE49-91C8AB54852C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B19E03-1359-BC4E-9981-4947C336A890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A6332151-AACC-E14E-B3DF-3D4980E70093}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{A6332151-AACC-E14E-B3DF-3D4980E70093}"/>
   </bookViews>
   <sheets>
     <sheet name="MA_DLD_MF_cases_new" sheetId="33" r:id="rId1"/>
-    <sheet name="MA_RD_MF_cases_new" sheetId="34" r:id="rId2"/>
-    <sheet name="All_data" sheetId="31" r:id="rId3"/>
-    <sheet name="MA_DLD_MF_case_new_same_control" sheetId="35" r:id="rId4"/>
+    <sheet name="MA_DLD_MF_cases_new_TEDS_new" sheetId="36" r:id="rId2"/>
+    <sheet name="MA_RD_MF_cases_new" sheetId="34" r:id="rId3"/>
+    <sheet name="MA_RD_MF_cases_new_TEDS_new" sheetId="37" r:id="rId4"/>
+    <sheet name="All_data" sheetId="31" r:id="rId5"/>
+    <sheet name="MA_DLD_MF_case_new_same_control" sheetId="35" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="31">
   <si>
     <t>Manchester</t>
   </si>
@@ -226,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,26 +252,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -278,22 +273,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22041CE8-1007-B941-8D24-DCB1ACEB9CF8}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="172" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,22 +609,22 @@
       <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -671,17 +651,17 @@
         <v>76</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" ref="H2:H14" si="0">D2/(D2+E2)</f>
+        <f t="shared" ref="H2" si="0">D2/(D2+E2)</f>
         <v>0.21052631578947367</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" ref="I2:I14" si="1">F2/(F2+G2)</f>
+        <f t="shared" ref="I2" si="1">F2/(F2+G2)</f>
         <v>0.16483516483516483</v>
       </c>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -743,7 +723,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1084,11 +1064,469 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3A2CA7-8869-6941-82CF-07CA9DE1F877}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8">
+        <v>8</v>
+      </c>
+      <c r="E2" s="8">
+        <v>30</v>
+      </c>
+      <c r="F2" s="8">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8">
+        <v>76</v>
+      </c>
+      <c r="H2" s="2">
+        <f t="shared" ref="H2:H14" si="0">D2/(D2+E2)</f>
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="I2" s="2">
+        <f t="shared" ref="I2:I14" si="1">F2/(F2+G2)</f>
+        <v>0.16483516483516483</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8">
+        <v>45</v>
+      </c>
+      <c r="E3" s="8">
+        <v>150</v>
+      </c>
+      <c r="F3" s="8">
+        <f>SUM(All_data!G10:G11)</f>
+        <v>89</v>
+      </c>
+      <c r="G3" s="8">
+        <f>SUM(All_data!H10:H11)</f>
+        <v>590</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13107511045655376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8">
+        <v>19</v>
+      </c>
+      <c r="E4" s="8">
+        <v>255</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9343065693430656E-2</v>
+      </c>
+      <c r="I4" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8">
+        <v>28</v>
+      </c>
+      <c r="E5" s="8">
+        <v>207</v>
+      </c>
+      <c r="F5" s="8">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11914893617021277</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12280701754385964</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>40</v>
+      </c>
+      <c r="E6" s="8">
+        <v>262</v>
+      </c>
+      <c r="F6" s="8">
+        <f>SUM(All_data!G24:G25)</f>
+        <v>98</v>
+      </c>
+      <c r="G6" s="8">
+        <f>SUM(All_data!H24:H25)</f>
+        <v>667</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13245033112582782</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12810457516339868</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8">
+        <v>25</v>
+      </c>
+      <c r="F7" s="8">
+        <v>15</v>
+      </c>
+      <c r="G7" s="8">
+        <v>76</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.24242424242424243</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16483516483516483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="8">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8">
+        <v>182</v>
+      </c>
+      <c r="F8" s="8">
+        <v>56</v>
+      </c>
+      <c r="G8" s="8">
+        <v>610</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10784313725490197</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>8.408408408408409E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8">
+        <f>SUM(All_data!E4:E7)</f>
+        <v>27</v>
+      </c>
+      <c r="E9" s="8">
+        <f>SUM(All_data!F4:F7)</f>
+        <v>214</v>
+      </c>
+      <c r="F9" s="8">
+        <f>SUM(All_data!G4:G5)</f>
+        <v>112</v>
+      </c>
+      <c r="G9" s="8">
+        <f>SUM(All_data!H4:H5)</f>
+        <v>749</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11203319502074689</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13008130081300814</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="8">
+        <v>21</v>
+      </c>
+      <c r="E10" s="8">
+        <v>136</v>
+      </c>
+      <c r="F10" s="8">
+        <v>49</v>
+      </c>
+      <c r="G10" s="8">
+        <v>389</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13375796178343949</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11187214611872145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8">
+        <v>34</v>
+      </c>
+      <c r="E11" s="8">
+        <v>187</v>
+      </c>
+      <c r="F11" s="8">
+        <v>143</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1031</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15384615384615385</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12180579216354344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8">
+        <v>31</v>
+      </c>
+      <c r="E12" s="8">
+        <v>203</v>
+      </c>
+      <c r="F12" s="8">
+        <v>136</v>
+      </c>
+      <c r="G12" s="8">
+        <v>914</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13247863247863248</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12952380952380951</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8">
+        <v>29</v>
+      </c>
+      <c r="E13" s="8">
+        <v>165</v>
+      </c>
+      <c r="F13" s="8">
+        <v>143</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1031</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14948453608247422</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12180579216354344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8">
+        <f>All_data!E2+All_data!E3</f>
+        <v>30</v>
+      </c>
+      <c r="E14" s="8">
+        <f>All_data!F2+All_data!F3</f>
+        <v>168</v>
+      </c>
+      <c r="F14" s="8">
+        <f>SUM(All_data!G4:G5)</f>
+        <v>112</v>
+      </c>
+      <c r="G14" s="8">
+        <f>SUM(All_data!H4:H5)</f>
+        <v>749</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13008130081300814</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E921E3C-C323-724D-A57D-7A5B65D2333E}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="172" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,22 +1541,22 @@
       <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1224,7 +1662,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1542,7 +1980,466 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEF8BF0-2A94-F241-8888-BE96A0DA741C}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView zoomScale="164" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8">
+        <f>SUM(All_data!E4:E5)</f>
+        <v>22</v>
+      </c>
+      <c r="E2" s="8">
+        <f>SUM(All_data!F4:F5)</f>
+        <v>169</v>
+      </c>
+      <c r="F2" s="8">
+        <f>SUM(All_data!G4:G5)</f>
+        <v>112</v>
+      </c>
+      <c r="G2" s="8">
+        <f>SUM(All_data!H4:H5)</f>
+        <v>749</v>
+      </c>
+      <c r="H2" s="2">
+        <f>D2/(D2+E2)</f>
+        <v>0.11518324607329843</v>
+      </c>
+      <c r="I2" s="2">
+        <f>F2/(F2+G2)</f>
+        <v>0.13008130081300814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8">
+        <f>SUM(All_data!E2:E3,All_data!E6,All_data!E7)</f>
+        <v>35</v>
+      </c>
+      <c r="E3" s="8">
+        <f>SUM(All_data!F2:F3,All_data!F6,All_data!F7)</f>
+        <v>213</v>
+      </c>
+      <c r="F3" s="8">
+        <f>SUM(All_data!G4:G5)</f>
+        <v>112</v>
+      </c>
+      <c r="G3" s="8">
+        <f>SUM(All_data!H4:H5)</f>
+        <v>749</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H14" si="0">D3/(D3+E3)</f>
+        <v>0.14112903225806453</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I14" si="1">F3/(F3+G3)</f>
+        <v>0.13008130081300814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8">
+        <v>22</v>
+      </c>
+      <c r="E4" s="8">
+        <v>182</v>
+      </c>
+      <c r="F4" s="8">
+        <v>56</v>
+      </c>
+      <c r="G4" s="8">
+        <v>610</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10784313725490197</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="1"/>
+        <v>8.408408408408409E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8">
+        <v>45</v>
+      </c>
+      <c r="E5" s="8">
+        <v>150</v>
+      </c>
+      <c r="F5" s="8">
+        <f>SUM(All_data!G10:G11)</f>
+        <v>89</v>
+      </c>
+      <c r="G5" s="8">
+        <f>SUM(All_data!H10:H11)</f>
+        <v>590</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13107511045655376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8">
+        <v>21</v>
+      </c>
+      <c r="E6" s="8">
+        <v>136</v>
+      </c>
+      <c r="F6" s="8">
+        <v>49</v>
+      </c>
+      <c r="G6" s="8">
+        <v>389</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13375796178343949</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11187214611872145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8">
+        <v>20</v>
+      </c>
+      <c r="E7" s="8">
+        <v>132</v>
+      </c>
+      <c r="F7" s="8">
+        <v>143</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1031</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13157894736842105</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12180579216354344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="8">
+        <v>43</v>
+      </c>
+      <c r="E8" s="8">
+        <v>218</v>
+      </c>
+      <c r="F8" s="8">
+        <v>143</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1031</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16475095785440613</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12180579216354344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="8">
+        <v>28</v>
+      </c>
+      <c r="E9" s="8">
+        <v>207</v>
+      </c>
+      <c r="F9" s="8">
+        <v>7</v>
+      </c>
+      <c r="G9" s="8">
+        <v>50</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11914893617021277</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12280701754385964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8">
+        <v>40</v>
+      </c>
+      <c r="E10" s="8">
+        <v>262</v>
+      </c>
+      <c r="F10" s="8">
+        <f>SUM(All_data!G24:G25)</f>
+        <v>98</v>
+      </c>
+      <c r="G10" s="8">
+        <f>SUM(All_data!H24:H25)</f>
+        <v>667</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13245033112582782</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12810457516339868</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8">
+        <v>5</v>
+      </c>
+      <c r="E11" s="8">
+        <v>14</v>
+      </c>
+      <c r="F11" s="8">
+        <v>15</v>
+      </c>
+      <c r="G11" s="8">
+        <v>76</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16483516483516483</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8">
+        <v>11</v>
+      </c>
+      <c r="E12" s="8">
+        <v>41</v>
+      </c>
+      <c r="F12" s="8">
+        <v>15</v>
+      </c>
+      <c r="G12" s="8">
+        <v>76</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21153846153846154</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16483516483516483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8">
+        <v>19</v>
+      </c>
+      <c r="E13" s="8">
+        <v>255</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9343065693430656E-2</v>
+      </c>
+      <c r="I13" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8">
+        <v>31</v>
+      </c>
+      <c r="E14" s="8">
+        <v>203</v>
+      </c>
+      <c r="F14" s="8">
+        <v>136</v>
+      </c>
+      <c r="G14" s="8">
+        <v>914</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13247863247863248</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12952380952380951</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CEA9B62-46B7-C34A-818B-01E939BEC29F}">
   <dimension ref="A1:J29"/>
   <sheetViews>
@@ -1565,16 +2462,16 @@
       <c r="D1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I1" s="9" t="s">
@@ -1929,16 +2826,16 @@
       <c r="D12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="16">
         <v>19</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="16">
         <v>189</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="16">
         <v>0</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="16">
         <v>0</v>
       </c>
       <c r="I12" s="10">
@@ -1997,16 +2894,16 @@
       <c r="D14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="11">
         <v>18</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="11">
         <v>97</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="11">
         <v>66</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="11">
         <v>450</v>
       </c>
       <c r="I14" s="10">
@@ -2065,10 +2962,10 @@
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="16">
         <v>15</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="16">
         <v>87</v>
       </c>
       <c r="G16" s="11">
@@ -2167,16 +3064,16 @@
       <c r="D19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19">
         <v>23</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19">
         <v>80</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19">
         <v>71</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19">
         <v>485</v>
       </c>
       <c r="I19" s="10">
@@ -2207,10 +3104,10 @@
       <c r="F20" s="11">
         <v>73</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20">
         <v>51</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20">
         <v>330</v>
       </c>
       <c r="I20" s="10">
@@ -2269,16 +3166,16 @@
       <c r="D22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="16">
         <v>16</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="16">
         <v>137</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="16">
         <v>4</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="16">
         <v>33</v>
       </c>
       <c r="I22" s="10">
@@ -2411,10 +3308,10 @@
       <c r="F26" s="11">
         <v>18</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="16">
         <v>11</v>
       </c>
-      <c r="H26" s="19">
+      <c r="H26" s="16">
         <v>37</v>
       </c>
       <c r="I26" s="10">
@@ -2479,10 +3376,10 @@
       <c r="F28" s="11">
         <v>18</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="16">
         <v>11</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="16">
         <v>37</v>
       </c>
       <c r="I28" s="10">
@@ -2533,7 +3430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE278C4-C422-1F45-A3E8-85E23634DC4D}">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -2553,22 +3450,22 @@
       <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2605,7 +3502,7 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -2667,7 +3564,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="7" t="s">

</xml_diff>